<commit_message>
sofia | test | error | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB5E153-BD86-480B-A574-C27FC132CCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B86AA7A-A2E2-4289-9003-5917D0EA96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="280">
   <si>
     <t>Форпик</t>
   </si>
@@ -514,9 +514,6 @@
   </si>
   <si>
     <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
   </si>
   <si>
     <t xml:space="preserve"> Статический крен от ветра              </t>
@@ -1419,31 +1416,31 @@
         <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -1467,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1496,15 +1493,15 @@
         <v>145</v>
       </c>
       <c r="E1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>273</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1517,10 +1514,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="20">
         <v>13163.9</v>
@@ -1537,7 +1534,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>148</v>
@@ -1557,7 +1554,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>148</v>
@@ -1578,10 +1575,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="20">
         <v>6.1909999999999998</v>
@@ -1598,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>148</v>
@@ -1627,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F8" s="9">
         <v>0.05</v>
@@ -1635,7 +1632,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -1648,7 +1645,7 @@
         <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>148</v>
@@ -1668,7 +1665,7 @@
         <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>148</v>
@@ -1688,7 +1685,7 @@
         <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>148</v>
@@ -1708,10 +1705,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>54</v>
@@ -1728,10 +1725,10 @@
         <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D14" s="20">
         <v>0</v>
@@ -1748,7 +1745,7 @@
         <v>144</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>148</v>
@@ -1766,10 +1763,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" t="s">
         <v>215</v>
-      </c>
-      <c r="B16" t="s">
-        <v>216</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -1786,10 +1783,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" t="s">
         <v>217</v>
-      </c>
-      <c r="B17" t="s">
-        <v>218</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>148</v>
@@ -1806,10 +1803,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
         <v>219</v>
-      </c>
-      <c r="B18" t="s">
-        <v>220</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -1826,10 +1823,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" t="s">
         <v>221</v>
-      </c>
-      <c r="B19" t="s">
-        <v>222</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>148</v>
@@ -1846,10 +1843,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" t="s">
         <v>223</v>
-      </c>
-      <c r="B20" t="s">
-        <v>224</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>148</v>
@@ -1866,10 +1863,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" t="s">
         <v>225</v>
-      </c>
-      <c r="B21" t="s">
-        <v>226</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>148</v>
@@ -1886,10 +1883,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" t="s">
         <v>227</v>
-      </c>
-      <c r="B22" t="s">
-        <v>228</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>148</v>
@@ -1906,10 +1903,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B23" t="s">
         <v>229</v>
-      </c>
-      <c r="B23" t="s">
-        <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>148</v>
@@ -1926,10 +1923,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" t="s">
         <v>231</v>
-      </c>
-      <c r="B24" t="s">
-        <v>232</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>148</v>
@@ -1946,10 +1943,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25" t="s">
         <v>233</v>
-      </c>
-      <c r="B25" t="s">
-        <v>234</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>148</v>
@@ -1966,10 +1963,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" t="s">
         <v>235</v>
-      </c>
-      <c r="B26" t="s">
-        <v>236</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>148</v>
@@ -1986,10 +1983,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
         <v>237</v>
-      </c>
-      <c r="B27" t="s">
-        <v>238</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>148</v>
@@ -2006,10 +2003,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" t="s">
         <v>239</v>
-      </c>
-      <c r="B28" t="s">
-        <v>240</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>148</v>
@@ -2026,10 +2023,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" t="s">
         <v>241</v>
-      </c>
-      <c r="B29" t="s">
-        <v>242</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>148</v>
@@ -2046,7 +2043,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -2059,10 +2056,10 @@
         <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="20">
         <v>19.655999999999999</v>
@@ -2079,10 +2076,10 @@
         <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>54</v>
@@ -2099,10 +2096,10 @@
         <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="20">
         <v>187.70599999999999</v>
@@ -2119,7 +2116,7 @@
         <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>148</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
@@ -2180,7 +2177,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>148</v>
@@ -2201,7 +2198,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>148</v>
@@ -2223,7 +2220,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>148</v>
@@ -2244,7 +2241,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>148</v>
@@ -2388,7 +2385,7 @@
         <v>109</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>54</v>
@@ -2408,7 +2405,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D48" s="20">
         <v>872.72799999999995</v>
@@ -2489,7 +2486,7 @@
         <v>119</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D52" s="20">
         <v>5.1710000000000003</v>
@@ -2509,7 +2506,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D53" s="20">
         <v>7.47</v>
@@ -2529,7 +2526,7 @@
         <v>123</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>54</v>
@@ -2549,7 +2546,7 @@
         <v>125</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>54</v>
@@ -2569,7 +2566,7 @@
         <v>127</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>54</v>
@@ -2589,7 +2586,7 @@
         <v>129</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>54</v>
@@ -2609,7 +2606,7 @@
         <v>131</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>54</v>
@@ -2629,7 +2626,7 @@
         <v>133</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D59" s="20">
         <v>28.058</v>
@@ -2649,7 +2646,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D60" s="20">
         <v>49.143999999999998</v>
@@ -2669,7 +2666,7 @@
         <v>137</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>54</v>
@@ -2689,7 +2686,7 @@
         <v>139</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D62" s="20">
         <v>565.29600000000005</v>
@@ -2709,7 +2706,7 @@
         <v>141</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>54</v>
@@ -2729,7 +2726,7 @@
         <v>143</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>54</v>
@@ -2755,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F65" s="9">
         <v>0.05</v>
@@ -2845,7 +2842,7 @@
         <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2864,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2881,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2898,7 +2895,7 @@
         <v>227.2</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2915,7 +2912,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2932,7 +2929,7 @@
         <v>240.2</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2949,7 +2946,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2983,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3000,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3017,7 +3014,7 @@
         <v>128.4</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3034,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3051,7 +3048,7 @@
         <v>109.3</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3068,7 +3065,7 @@
         <v>129.9</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3085,7 +3082,7 @@
         <v>129.9</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3102,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3119,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3136,7 +3133,7 @@
         <v>97.5</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3153,7 +3150,7 @@
         <v>97.5</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3170,7 +3167,7 @@
         <v>265.7</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,7 +3184,7 @@
         <v>265.7</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3204,7 +3201,7 @@
         <v>206.4</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3221,7 +3218,7 @@
         <v>217.2</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3238,7 +3235,7 @@
         <v>6.6</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3255,7 +3252,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,7 +3269,7 @@
         <v>7.8</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3289,7 +3286,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3306,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3323,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3340,7 +3337,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3357,7 +3354,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3374,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3391,7 +3388,7 @@
         <v>17</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3408,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3425,7 +3422,7 @@
         <v>0.5</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3442,7 +3439,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3459,7 +3456,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3476,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3493,7 +3490,7 @@
         <v>1.8</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3510,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3527,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,7 +3541,7 @@
         <v>0.4</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,7 +3558,7 @@
         <v>6.7</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,7 +3575,7 @@
         <v>0.3</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3646,7 +3643,7 @@
         <v>8.4</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3663,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3680,7 +3677,7 @@
         <v>6</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3697,7 +3694,7 @@
         <v>3.6</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,7 +3711,7 @@
         <v>3.6</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3731,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3782,7 +3779,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>54</v>
@@ -3795,12 +3792,12 @@
         <v>900.2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>54</v>
@@ -3813,12 +3810,12 @@
         <v>51.3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>54</v>
@@ -3831,12 +3828,12 @@
         <v>617.70000000000005</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>54</v>
@@ -3849,12 +3846,12 @@
         <v>51.3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>54</v>
@@ -3867,12 +3864,12 @@
         <v>256.39999999999998</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>54</v>
@@ -3885,12 +3882,12 @@
         <v>51.3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>54</v>
@@ -3903,12 +3900,12 @@
         <v>1493.5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>54</v>
@@ -3921,12 +3918,12 @@
         <v>988.3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>54</v>
@@ -3939,12 +3936,12 @@
         <v>51.3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -3957,12 +3954,12 @@
         <v>244.5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>54</v>
@@ -3975,12 +3972,12 @@
         <v>51.3</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>54</v>
@@ -3993,12 +3990,12 @@
         <v>912.7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>54</v>
@@ -4011,12 +4008,12 @@
         <v>51.3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>54</v>
@@ -4029,12 +4026,12 @@
         <v>748.7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>54</v>
@@ -4047,12 +4044,12 @@
         <v>51.3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>54</v>
@@ -4065,12 +4062,12 @@
         <v>408.6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>54</v>
@@ -4083,12 +4080,12 @@
         <v>51.3</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -4101,7 +4098,7 @@
         <v>493.3</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4155,7 +4152,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4163,7 +4160,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4524,22 +4521,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>179</v>
-      </c>
       <c r="E1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>273</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4656,22 +4653,22 @@
         <v>60</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>273</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>274</v>
       </c>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" s="9">
         <v>53.16</v>
@@ -4688,7 +4685,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="9">
         <v>53.16</v>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="9">
         <v>36.36</v>
@@ -4722,7 +4719,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5" s="9">
         <v>36.36</v>
@@ -4766,10 +4763,10 @@
         <v>153</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>273</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5075,8 +5072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500720D-7F16-4373-97E5-9F957C7E1B58}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5091,22 +5088,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>145</v>
       </c>
       <c r="E1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>273</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5117,7 +5114,7 @@
         <v>155</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>54</v>
@@ -5137,19 +5134,19 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="9">
         <v>1</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>156</v>
@@ -5160,10 +5157,10 @@
         <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="19">
         <v>0.105</v>
@@ -5183,10 +5180,10 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>54</v>
@@ -5206,10 +5203,10 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="19">
         <v>0.20699999999999999</v>
@@ -5229,10 +5226,10 @@
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="19">
         <v>0.10199999999999999</v>
@@ -5252,7 +5249,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>148</v>
@@ -5275,7 +5272,7 @@
         <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>148</v>
@@ -5298,7 +5295,7 @@
         <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>148</v>
@@ -5321,19 +5318,19 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="19">
         <v>53.555999999999997</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="9">
         <v>1</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="G11" t="s">
         <v>156</v>
@@ -5344,19 +5341,19 @@
         <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="9">
         <v>1</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>156</v>
@@ -5367,7 +5364,7 @@
         <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>148</v>
@@ -5390,10 +5387,10 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>54</v>
@@ -5413,19 +5410,19 @@
         <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="9">
         <v>1</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="G15" t="s">
         <v>156</v>
@@ -5436,19 +5433,19 @@
         <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D16" s="19">
         <v>4.0910000000000002</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="9">
         <v>1</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="G16" t="s">
         <v>156</v>
@@ -5459,10 +5456,10 @@
         <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D17" s="19">
         <v>0.182</v>
@@ -5482,7 +5479,7 @@
         <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
sofia | test2 | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638DC193-F43D-447C-BCE7-3A6341554FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA8CE15-E0C2-4D65-81A5-D33735186C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="281">
   <si>
     <t>Форпик</t>
   </si>
@@ -986,7 +986,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -1070,6 +1070,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1392,7 +1395,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1445,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="30" t="s">
         <v>246</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1470,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2494,8 +2497,8 @@
       <c r="C52" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D52" s="20">
-        <v>5.1710000000000003</v>
+      <c r="D52" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>54</v>
@@ -2514,8 +2517,8 @@
       <c r="C53" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D53" s="20">
-        <v>7.47</v>
+      <c r="D53" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>54</v>
@@ -2775,7 +2778,7 @@
         <v>148</v>
       </c>
       <c r="D66" s="20">
-        <v>63.933</v>
+        <v>61.433999999999997</v>
       </c>
       <c r="E66" s="9">
         <v>1</v>
@@ -5100,7 +5103,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5282,7 +5285,7 @@
         <v>148</v>
       </c>
       <c r="D8" s="19">
-        <v>0.47199999999999998</v>
+        <v>0.91379999999999995</v>
       </c>
       <c r="E8" s="9">
         <v>5</v>
@@ -5397,7 +5400,7 @@
         <v>148</v>
       </c>
       <c r="D13" s="19">
-        <v>5.7099999999999998E-2</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
sofia | test2 | density | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC478BBE-8A6E-4420-9042-6A292C04796B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59B6F8-EBC0-4B29-A58C-5DB9E148945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3736,7 +3736,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,8 +3773,8 @@
         <v>264</v>
       </c>
       <c r="C2" s="8">
-        <f>1/0.54449</f>
-        <v>1.8365810207717312</v>
+        <f>1/0.543295147</f>
+        <v>1.8406201592667639</v>
       </c>
       <c r="D2" s="3">
         <v>3421.7</v>
@@ -3791,8 +3791,8 @@
         <v>266</v>
       </c>
       <c r="C3" s="8">
-        <f>1/0.54449</f>
-        <v>1.8365810207717312</v>
+        <f>1/0.543295147</f>
+        <v>1.8406201592667639</v>
       </c>
       <c r="D3" s="3">
         <v>4052.6</v>

</xml_diff>